<commit_message>
added solar panel and super capacitor
</commit_message>
<xml_diff>
--- a/AEMBLINK-R1.1-BOM.xlsx
+++ b/AEMBLINK-R1.1-BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43844AFB-82A7-41C5-AA85-9DF5CD07630F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E7F3B0-F039-4869-916F-F73FDA025352}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
   <si>
     <t>10uF</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Changed R4 from 20R to 33R</t>
+  </si>
+  <si>
+    <t>super capacitor</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>1V 80mA 30x25mm</t>
   </si>
 </sst>
 </file>
@@ -672,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,6 +1392,76 @@
         <v>27</v>
       </c>
       <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R17" xr:uid="{46A2BD4D-A1CD-422D-8EA6-D0EDA41FD651}">

</xml_diff>